<commit_message>
update A01 readme and materials
</commit_message>
<xml_diff>
--- a/01-point_clouds_labeling/data arrangement.xlsx
+++ b/01-point_clouds_labeling/data arrangement.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1-PhD work\z-Temp work\Course-TA\TBA 4256\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2-PhD course\3D digital modeling\clean_codes\01-point_clouds_labeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F3AB00-65D0-4EF0-ACDC-69EF6DF704D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1306CB0C-3300-4691-875D-A2EE25E63904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33490" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>No.</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>32-1-510-213-15</t>
-  </si>
-  <si>
-    <t>a little many</t>
   </si>
 </sst>
 </file>
@@ -191,33 +188,15 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -242,6 +221,24 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -256,12 +253,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{466570E4-0011-4940-AE81-983355FB02C2}" name="Table1" displayName="Table1" ref="A1:C31" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{466570E4-0011-4940-AE81-983355FB02C2}" name="Table1" displayName="Table1" ref="A1:C31" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:C31" xr:uid="{466570E4-0011-4940-AE81-983355FB02C2}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D7EE242C-CBF9-4469-A1A3-36A32C66700C}" name="No."/>
     <tableColumn id="2" xr3:uid="{2C2BC8B3-B9A7-4988-AF89-B18CCC17DEA3}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{1A668D1F-3BA3-4E8F-9083-258E2F327AAF}" name="Data id (kartid)" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{1A668D1F-3BA3-4E8F-9083-258E2F327AAF}" name="Data id (kartid)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -532,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,7 +676,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -687,7 +684,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -695,7 +692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -703,7 +700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -711,7 +708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -719,7 +716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -727,7 +724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -735,7 +732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -743,7 +740,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -751,7 +748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -759,7 +756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -767,7 +764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -775,7 +772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -783,7 +780,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -791,15 +788,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D31" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>